<commit_message>
update(demo files): Update excel files with the correct format of the cells
</commit_message>
<xml_diff>
--- a/gearshift/demos/gs_input_demo_empty.xlsx
+++ b/gearshift/demos/gs_input_demo_empty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\European Comision\WLTP\gearshift_calculation_tool\gearshift\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A18F04F-F60A-4021-8E1A-D448C997A111}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BFEEB7-91B3-49EA-A967-AC9BFB417528}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="1380" windowWidth="31755" windowHeight="18030" xr2:uid="{5C24A396-E983-DB47-8B10-835CCBF80F80}"/>
+    <workbookView xWindow="3630" yWindow="1965" windowWidth="31755" windowHeight="18030" xr2:uid="{5C24A396-E983-DB47-8B10-835CCBF80F80}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -20,15 +20,24 @@
     <sheet name="gearbox_ratios" sheetId="11" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="case" localSheetId="1">case!$A$1:$Z$127</definedName>
+    <definedName name="case" localSheetId="1">case!$A$1:$Z$3</definedName>
     <definedName name="engine" localSheetId="3">engine!$A$1:$D$5097</definedName>
     <definedName name="gearbox" localSheetId="4">gearbox_ratios!$A$1:$C$652</definedName>
     <definedName name="vehicle" localSheetId="2">vehicle!$A$1:$K$118</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -304,18 +313,7 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Welcome to the Gearshift calculation tool (GS) declaration file.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="0"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -326,6 +324,17 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Welcome to the Gearshift calculation tool (GS) declaration file.</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="0"/>
         <rFont val="Calibri"/>
@@ -333,7 +342,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-All the inputs required to denerare the declaration file with JET are provided through this file.
+All the inputs required to generate the input file for the Gearshift Tool are provided through this file.
 Tabs marked in </t>
     </r>
     <r>
@@ -350,25 +359,13 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <i/>
         <sz val="12"/>
         <color theme="0"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">are fixed values used by the tool, these values must not be changed unless a type of check is to be carried out.
+      <t xml:space="preserve"> are fixed values used by the tool, these values must not be changed unless a type of check is to be carried out.
 Tabs marked in </t>
     </r>
     <r>
@@ -392,23 +389,16 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> are mandatory depending on the vehicle configuration and the test.
-The</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri (Cuerpo)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+The </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <i/>
         <sz val="12"/>
         <color rgb="FFFFC000"/>
-        <rFont val="Calibri (Cuerpo)_x0000_"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>case tab</t>
     </r>
@@ -428,7 +418,9 @@
         <b/>
         <sz val="12"/>
         <color rgb="FFFFC000"/>
-        <rFont val="Calibri (Cuerpo)_x0000_"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>vehicle tab</t>
     </r>
@@ -440,7 +432,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> tab is required. The vehicle contains the all information relative to the vehicle.
+      <t xml:space="preserve"> tab is required. The vehicle contains all information relative to the vehicle.
 The </t>
     </r>
     <r>
@@ -452,15 +444,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">gear_box_ratios tab </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0"/>
-        <rFont val="Calibri (Cuerpo)_x0000_"/>
-      </rPr>
-      <t>contains the gearbox ratios of each vehicle</t>
+      <t>gear_box_ratios</t>
     </r>
     <r>
       <rPr>
@@ -470,29 +454,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">.
-The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>engine tab</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  is required. The engine contains the all information relative to the full power curve.
+      <t xml:space="preserve"> tab contains the gearbox ratios of each vehicle.
+The engine tab is required. The engine contains all information relative to the full power curve.
 </t>
     </r>
   </si>
@@ -501,7 +464,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -540,26 +503,9 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <i/>
       <sz val="12"/>
       <color rgb="FFFFFF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -589,29 +535,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFFC000"/>
-      <name val="Calibri (Cuerpo)_x0000_"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FFFFC000"/>
-      <name val="Calibri (Cuerpo)_x0000_"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFFC000"/>
-      <name val="Calibri (Cuerpo)_x0000_"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri (Cuerpo)_x0000_"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -623,9 +546,15 @@
       <name val="Calibri (Cuerpo)_x0000_"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="14"/>
-      <color rgb="FFFFC000"/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -664,21 +593,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -698,7 +627,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -707,8 +636,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -795,23 +727,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>86</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CuadroTexto 1">
+        <xdr:cNvPr id="3" name="CuadroTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCA0E042-C39A-0648-811D-CB539EDE8828}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{377648B4-0529-4ADD-B2DE-651C2D6DBF65}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -819,8 +751,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17119600" y="215900"/>
-          <a:ext cx="8255000" cy="17272000"/>
+          <a:off x="17430750" y="200025"/>
+          <a:ext cx="8382000" cy="17002125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -860,6 +792,72 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
+            <a:t>- case:  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Integer</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> parameter to define the case number of the execution.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>vehicle:  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>String parameter to define the vehicle code. Please check that this parameter should be exactly the same in all sheets.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>-</a:t>
           </a:r>
           <a:r>
@@ -876,10 +874,18 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>calc_dsc:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
+            <a:t>calc_dsc: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
@@ -887,19 +893,89 @@
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>This</a:t>
-          </a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>is a logical scalar (0 = No | 1 = Yes) , specifying</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>if the calculated downscaling value shall be used instead of the</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>the value given by the input parameter Downscaling Percentage. If the value is 1,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> the downscaling factor will be calculated following the Paragraph 8.3. of Sub-Annex 1. If the value is 0, the downscaling factor defined in the  f_dsc parameter will be used.</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
+            <a:t>- Apply Downscaling </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(do_dsc): This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t> </a:t>
           </a:r>
           <a:r>
@@ -908,7 +984,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>is a logical scalar, specifying</a:t>
+            <a:t>is a logical scalar (0 = No | 1 = Yes) , specifying if the trace shall</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
@@ -924,7 +1000,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>if the calculated downscaling value shall be used instead of the</a:t>
+            <a:t>be downscaled. [Ref:</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
@@ -932,6 +1008,52 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
+            <a:t> Paragraph 8 of Sub-Annex 1]</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- Apply Speed Cap </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(do_cap):</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t> </a:t>
           </a:r>
           <a:r>
@@ -940,7 +1062,23 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>the value given by the input parameter Downscaling Percentage.</a:t>
+            <a:t>is a logical scalar (0 = No | 1 = Yes) , specifying if the trace shall be</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>capped to the given CappedSpeed. [Ref: Paragraph 9.1 of Sub-Annex 1]</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -957,141 +1095,6 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>- Apply Downscaling </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(do_dsc): This</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>is a logical scalar, specifying if the trace shall</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>be downscaled. [Ref:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Paragraph 8 of Sub-Annex 1]</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- Apply Speed Cap </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(do_cap):</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> This</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>is a logical scalar, specifying if the trace shall be</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>capped to the given CappedSpeed. [Ref: Paragraph 9.1 of Sub-Annex 1]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
             <a:t>Apply Distance Compensation </a:t>
           </a:r>
           <a:r>
@@ -1108,7 +1111,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> ApplyDistanceCompensation is a logical scalar, specifying it the trace shall be compensated for distance due to capped speeds. [Ref: Paragraph 9.2.1 of Sub-Annex 1]</a:t>
+            <a:t> ApplyDistanceCompensation is a logical scalar (0 = No | 1 = Yes) , specifying it the trace shall be compensated for distance due to capped speeds. [Ref: Paragraph 9.2.1 of Sub-Annex 1]</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4000,7 +4003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3C2E93-7C6E-7147-8A63-5B38643369BA}">
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:O50"/>
     </sheetView>
   </sheetViews>
@@ -4254,598 +4257,598 @@
       <c r="A16" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
     </row>
     <row r="17" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
     </row>
     <row r="18" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
     </row>
     <row r="19" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
     </row>
     <row r="20" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
     </row>
     <row r="21" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
     </row>
     <row r="22" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
     </row>
     <row r="23" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
     </row>
     <row r="24" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
     </row>
     <row r="25" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
     </row>
     <row r="26" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
     </row>
     <row r="27" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
     </row>
     <row r="28" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
     </row>
     <row r="29" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
     </row>
     <row r="30" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
     </row>
     <row r="31" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
     </row>
     <row r="32" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
     </row>
     <row r="33" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
     </row>
     <row r="34" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
     </row>
     <row r="35" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
     </row>
     <row r="36" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
     </row>
     <row r="37" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
     </row>
     <row r="38" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
     </row>
     <row r="39" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
     </row>
     <row r="40" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
     </row>
     <row r="41" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
     </row>
     <row r="42" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
     </row>
     <row r="43" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
     </row>
     <row r="44" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
     </row>
     <row r="45" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
     </row>
     <row r="46" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
     </row>
     <row r="47" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+      <c r="O47" s="19"/>
     </row>
     <row r="48" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="18"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
     </row>
     <row r="49" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="18"/>
-      <c r="M49" s="18"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="18"/>
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
+      <c r="O49" s="19"/>
     </row>
     <row r="50" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
-      <c r="N50" s="18"/>
-      <c r="O50" s="18"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
     </row>
     <row r="51" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A51" s="6"/>
@@ -4995,10 +4998,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD41"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -5017,7 +5020,7 @@
     <col min="13" max="14" width="8.375" style="11" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="8.875" style="11" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="9.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.125" style="11" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="6.5" style="11" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7" style="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.375" style="11" bestFit="1" customWidth="1"/>
@@ -5111,7 +5114,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>53</v>
@@ -5185,6 +5188,9 @@
       <c r="Z2" s="16" t="s">
         <v>52</v>
       </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="S3" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5200,7 +5206,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD41"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -5253,7 +5259,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>33</v>
@@ -5301,7 +5307,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A777" sqref="A777:XFD1156"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -5328,7 +5334,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>34</v>
@@ -5341,6 +5347,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5354,7 +5361,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -5377,7 +5384,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
update(demo): Block format of different sheets of the empty input template
</commit_message>
<xml_diff>
--- a/gearshift/demos/gs_input_demo_empty.xlsx
+++ b/gearshift/demos/gs_input_demo_empty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\European Comision\WLTP\gearshift_calculation_tool\gearshift\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BFEEB7-91B3-49EA-A967-AC9BFB417528}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41345ADE-7E52-4382-85B1-811E69469DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="1965" windowWidth="31755" windowHeight="18030" xr2:uid="{5C24A396-E983-DB47-8B10-835CCBF80F80}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5C24A396-E983-DB47-8B10-835CCBF80F80}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -20,10 +20,10 @@
     <sheet name="gearbox_ratios" sheetId="11" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="case" localSheetId="1">case!$A$1:$Z$3</definedName>
+    <definedName name="case" localSheetId="1">case!$A$1:$V$3</definedName>
     <definedName name="engine" localSheetId="3">engine!$A$1:$D$5097</definedName>
     <definedName name="gearbox" localSheetId="4">gearbox_ratios!$A$1:$C$652</definedName>
-    <definedName name="vehicle" localSheetId="2">vehicle!$A$1:$K$118</definedName>
+    <definedName name="vehicle" localSheetId="2">vehicle!$A$1:$J$118</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -122,24 +122,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>case</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> do_dsc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> do_cap</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> do_cmp</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> calc_dsc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> f_dsc</t>
   </si>
   <si>
     <t xml:space="preserve"> v_cap</t>
@@ -284,9 +269,6 @@
     <t>%</t>
   </si>
   <si>
-    <t>SM</t>
-  </si>
-  <si>
     <t>f2</t>
   </si>
   <si>
@@ -312,13 +294,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">
 </t>
     </r>
@@ -365,7 +340,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> are fixed values used by the tool, these values must not be changed unless a type of check is to be carried out.
+      <t xml:space="preserve"> are mandatory depending on the vehicle configuration and the test.
 Tabs marked in </t>
     </r>
     <r>
@@ -388,14 +363,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> are mandatory depending on the vehicle configuration and the test.
+      <t xml:space="preserve"> are optional sheets and values.
 The </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FFFFC000"/>
+        <color rgb="FFFFFF00"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -411,13 +386,23 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> has to be necessarily filled in to calculate gearshift values. This tab contains information regarding the simulated vehicle: characteristics of the engine, downscaling factor, capped speed, engine speed.
-The </t>
+The</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FFFFC000"/>
+        <color rgb="FFFFFF00"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -433,13 +418,23 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> tab is required. The vehicle contains all information relative to the vehicle.
-The </t>
+The</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FFFFC000"/>
+        <color rgb="FFFFFF00"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -449,22 +444,55 @@
     <r>
       <rPr>
         <sz val="12"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
         <color theme="0"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> tab contains the gearbox ratios of each vehicle.
-The engine tab is required. The engine contains all information relative to the full power curve.
+      <t xml:space="preserve"> contains the gearbox ratios of each vehicle.
+The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>engine tab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is required. The engine contains all information relative to the full power curve.
 </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> v_max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -520,14 +548,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFFC000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -559,8 +579,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,6 +614,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -593,57 +634,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -727,16 +805,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -751,8 +829,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17430750" y="200025"/>
-          <a:ext cx="8382000" cy="17002125"/>
+          <a:off x="15135225" y="200026"/>
+          <a:ext cx="8382000" cy="15430500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -792,7 +870,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>- case:  </a:t>
+            <a:t>case:  </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
@@ -820,14 +898,6 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- </a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
@@ -845,7 +915,7 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="1">
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
             <a:solidFill>
               <a:schemeClr val="bg1"/>
             </a:solidFill>
@@ -853,315 +923,20 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>-</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>calc_dsc: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>This</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>is a logical scalar (0 = No | 1 = Yes) , specifying</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>if the calculated downscaling value shall be used instead of the</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>the value given by the input parameter Downscaling Percentage. If the value is 1,</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> the downscaling factor will be calculated following the Paragraph 8.3. of Sub-Annex 1. If the value is 0, the downscaling factor defined in the  f_dsc parameter will be used.</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- Apply Downscaling </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(do_dsc): This</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>is a logical scalar (0 = No | 1 = Yes) , specifying if the trace shall</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>be downscaled. [Ref:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Paragraph 8 of Sub-Annex 1]</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- Apply Speed Cap </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(do_cap):</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> This</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>is a logical scalar (0 = No | 1 = Yes) , specifying if the trace shall be</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>capped to the given CappedSpeed. [Ref: Paragraph 9.1 of Sub-Annex 1]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Apply Distance Compensation </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(do_cmp):</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> ApplyDistanceCompensation is a logical scalar (0 = No | 1 = Yes) , specifying it the trace shall be compensated for distance due to capped speeds. [Ref: Paragraph 9.2.1 of Sub-Annex 1]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Use Calculated Downscaling Percentage </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(calc_dsc): This is a logical scalar, specifying if the calculated downscaling value shall be used instead of the the value given by the input parameter DownscalingPercentage. [Ref: Paragraph 8.2 of Sub-Annex 1]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Downscaling Percentage </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(f_dsc): This is a double scalar, specifying the degree of  downscaling. This value will only be used if the input parameter Use Calculated Downscaling Percentage is false. [Ref: Paragraph 8.2 of Sub-Annex 1]</a:t>
+            <a:t>Maximum velocity </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(v_max): The maximum velocity declared by the manofacturer.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1979,16 +1754,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>177801</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2003,8 +1778,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7791450" y="377825"/>
-          <a:ext cx="6731000" cy="7089775"/>
+          <a:off x="7324725" y="377826"/>
+          <a:ext cx="6731000" cy="6394450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2761,103 +2536,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Safety Margin</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> (</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>SM):</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>The safety margin is accounting for the difference</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>between the stationary full load condition power curve</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>and the power available during transition conditions.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>SM is set to 10 per cent. [Ref:Paragraph 3.4 of Sub-Annex 2]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
           <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0">
             <a:solidFill>
               <a:schemeClr val="bg1"/>
@@ -2899,13 +2577,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>200024</xdr:rowOff>
+      <xdr:rowOff>200023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2920,8 +2598,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3152775" y="600074"/>
-          <a:ext cx="5029200" cy="2066926"/>
+          <a:off x="3152775" y="600073"/>
+          <a:ext cx="5029200" cy="2266951"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3124,6 +2802,13 @@
             </a:rPr>
             <a:t>[Ref: Paragraph 2, point h of Sub-Annex 2]</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -4009,981 +3694,981 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="15" width="9.125" style="8" customWidth="1"/>
-    <col min="16" max="16" width="9.125" style="3" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.125" style="3" hidden="1"/>
+    <col min="1" max="15" width="9.125" style="17" customWidth="1"/>
+    <col min="16" max="16" width="9.125" style="16" hidden="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.125" style="16" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="1:15" s="8" customFormat="1"/>
-    <row r="16" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-    </row>
-    <row r="17" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-    </row>
-    <row r="18" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-    </row>
-    <row r="19" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-    </row>
-    <row r="20" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-    </row>
-    <row r="21" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-    </row>
-    <row r="22" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-    </row>
-    <row r="23" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-    </row>
-    <row r="24" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-    </row>
-    <row r="25" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-    </row>
-    <row r="26" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
-    </row>
-    <row r="27" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-    </row>
-    <row r="28" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-    </row>
-    <row r="29" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
-    </row>
-    <row r="30" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-    </row>
-    <row r="31" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-    </row>
-    <row r="32" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-    </row>
-    <row r="33" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-    </row>
-    <row r="34" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-    </row>
-    <row r="35" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A35" s="19"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
-    </row>
-    <row r="36" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
-    </row>
-    <row r="37" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-    </row>
-    <row r="38" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-    </row>
-    <row r="39" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
-    </row>
-    <row r="40" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
-    </row>
-    <row r="41" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
-    </row>
-    <row r="42" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
-    </row>
-    <row r="43" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
-      <c r="N43" s="19"/>
-      <c r="O43" s="19"/>
-    </row>
-    <row r="44" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
-    </row>
-    <row r="45" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
-    </row>
-    <row r="46" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="19"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19"/>
-      <c r="O46" s="19"/>
-    </row>
-    <row r="47" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A47" s="19"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
-      <c r="L47" s="19"/>
-      <c r="M47" s="19"/>
-      <c r="N47" s="19"/>
-      <c r="O47" s="19"/>
-    </row>
-    <row r="48" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="19"/>
-      <c r="M48" s="19"/>
-      <c r="N48" s="19"/>
-      <c r="O48" s="19"/>
-    </row>
-    <row r="49" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
-      <c r="J49" s="19"/>
-      <c r="K49" s="19"/>
-      <c r="L49" s="19"/>
-      <c r="M49" s="19"/>
-      <c r="N49" s="19"/>
-      <c r="O49" s="19"/>
-    </row>
-    <row r="50" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A50" s="19"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-      <c r="K50" s="19"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="19"/>
-      <c r="N50" s="19"/>
-      <c r="O50" s="19"/>
-    </row>
-    <row r="51" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-    </row>
-    <row r="52" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="6"/>
-      <c r="O52" s="6"/>
-    </row>
-    <row r="53" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-      <c r="M53" s="6"/>
-      <c r="N53" s="6"/>
-      <c r="O53" s="6"/>
-    </row>
-    <row r="54" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
-      <c r="M54" s="6"/>
-      <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
-    </row>
-    <row r="55" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
-    </row>
-    <row r="56" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="6"/>
-      <c r="O56" s="6"/>
-    </row>
-    <row r="57" spans="1:15" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="7"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+    </row>
+    <row r="15" spans="1:15" s="17" customFormat="1"/>
+    <row r="16" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+    </row>
+    <row r="17" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+    </row>
+    <row r="18" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+    </row>
+    <row r="19" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+    </row>
+    <row r="20" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+    </row>
+    <row r="21" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+    </row>
+    <row r="22" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+    </row>
+    <row r="23" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+    </row>
+    <row r="24" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+    </row>
+    <row r="25" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+    </row>
+    <row r="26" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+    </row>
+    <row r="27" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+    </row>
+    <row r="28" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+    </row>
+    <row r="29" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+    </row>
+    <row r="30" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+    </row>
+    <row r="31" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+    </row>
+    <row r="32" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+    </row>
+    <row r="33" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+    </row>
+    <row r="34" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+    </row>
+    <row r="35" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+    </row>
+    <row r="36" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
+    </row>
+    <row r="37" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="23"/>
+    </row>
+    <row r="38" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23"/>
+    </row>
+    <row r="39" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="23"/>
+    </row>
+    <row r="40" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A40" s="23"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="23"/>
+    </row>
+    <row r="41" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A41" s="23"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
+    </row>
+    <row r="42" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A42" s="23"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="23"/>
+    </row>
+    <row r="43" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+    </row>
+    <row r="44" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="23"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="23"/>
+    </row>
+    <row r="45" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="23"/>
+    </row>
+    <row r="46" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
+      <c r="O46" s="23"/>
+    </row>
+    <row r="47" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="23"/>
+      <c r="N47" s="23"/>
+      <c r="O47" s="23"/>
+    </row>
+    <row r="48" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="23"/>
+      <c r="N48" s="23"/>
+      <c r="O48" s="23"/>
+    </row>
+    <row r="49" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="23"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="23"/>
+    </row>
+    <row r="50" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A50" s="23"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="23"/>
+      <c r="L50" s="23"/>
+      <c r="M50" s="23"/>
+      <c r="N50" s="23"/>
+      <c r="O50" s="23"/>
+    </row>
+    <row r="51" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A51" s="19"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19"/>
+    </row>
+    <row r="52" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="19"/>
+    </row>
+    <row r="53" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A53" s="19"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="19"/>
+      <c r="O53" s="19"/>
+    </row>
+    <row r="54" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A54" s="19"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="19"/>
+      <c r="N54" s="19"/>
+      <c r="O54" s="19"/>
+    </row>
+    <row r="55" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A55" s="19"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19"/>
+      <c r="M55" s="19"/>
+      <c r="N55" s="19"/>
+      <c r="O55" s="19"/>
+    </row>
+    <row r="56" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
+      <c r="A56" s="19"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="19"/>
+      <c r="N56" s="19"/>
+      <c r="O56" s="19"/>
+    </row>
+    <row r="57" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A57" s="20"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="20"/>
+      <c r="N57" s="20"/>
+      <c r="O57" s="20"/>
     </row>
     <row r="61" spans="1:15" hidden="1">
-      <c r="B61" s="9"/>
+      <c r="B61" s="1"/>
     </row>
     <row r="62" spans="1:15" hidden="1">
-      <c r="B62" s="9"/>
+      <c r="B62" s="1"/>
     </row>
     <row r="63" spans="1:15" hidden="1">
-      <c r="B63" s="9"/>
+      <c r="B63" s="1"/>
     </row>
     <row r="64" spans="1:15" hidden="1">
-      <c r="B64" s="9"/>
+      <c r="B64" s="1"/>
     </row>
     <row r="65" ht="15" customHeight="1"/>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A16:O50"/>
   </mergeCells>
@@ -4996,9 +4681,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5411BEF-2978-8443-BBBB-A7CA880230E3}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -5006,204 +4691,177 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.875" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="8.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.875" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="6.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="6.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:22" s="4" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" s="2" customFormat="1">
-      <c r="A2" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="16" t="s">
+    </row>
+    <row r="2" spans="1:22" s="6" customFormat="1">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="U2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="V2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="X2" s="16" t="s">
+      <c r="Q2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z2" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
-      <c r="S3" s="10"/>
+      <c r="R2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" scenarios="1" insertRows="0"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C36EDB-F1C1-C34B-BB09-98901FF0C272}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -5211,98 +4869,96 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="10" customFormat="1">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" s="8" customFormat="1">
+      <c r="A1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="H2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="I2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>47</v>
-      </c>
+    </row>
+    <row r="37" spans="8:8">
+      <c r="H37" s="13"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" scenarios="1" insertRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DD5A06-A180-B048-9A2E-BB46AFCD04AB}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -5312,42 +4968,44 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>46</v>
+      <c r="A1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>47</v>
+      <c r="A2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <sheetProtection sheet="1" scenarios="1"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5356,7 +5014,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF7C22E-9A75-AE47-84D0-F58349538173}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -5366,34 +5024,36 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>43</v>
+      <c r="B2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update(empty demo): Update empty demo file.
</commit_message>
<xml_diff>
--- a/gearshift/demos/gs_input_demo_empty.xlsx
+++ b/gearshift/demos/gs_input_demo_empty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\European Comision\WLTP\gearshift_calculation_tool\gearshift\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41345ADE-7E52-4382-85B1-811E69469DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FE6E65-CA44-438E-880F-596B37793F17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5C24A396-E983-DB47-8B10-835CCBF80F80}"/>
   </bookViews>
@@ -2837,6 +2837,271 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>200023</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CuadroTexto 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{319ED4E8-22E7-460A-B4ED-B3358EE92B40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3152775" y="600073"/>
+          <a:ext cx="5029200" cy="2266951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="16355C"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>FullPowerCurve</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>n ==&gt; P_wot(n), ASM):</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>The full load power curve over the engine speed range.The power curve shall consist of a sufficient number of data sets (n,Pwot)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>so that the calculation of interim points between consecutive data sets</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>can be performed by linear interpolation.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ASM is an additional power safety margin,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>which may be applied at the request of the manufacturer.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>It will be defined by an additional column of FullPowerCurve</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>since regulation ECE-TRANS-WP29-GRPE-2017-07.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>n,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> p </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>[Ref: Paragraph 2, point h of Sub-Annex 2]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ASM </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>[Ref: Paragraph 3.4 of Sub-Annex 2]</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3329,6 +3594,534 @@
                   </a:solidFill>
                   <a:effectLst/>
                   <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑣)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t> shall be calculated using the equations in paragraph 8. of Sub-Annex 7; [Ref: Paragraph 2, point e of Sub-Annex 2]</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="CuadroTexto 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BB209E8-E9D6-4FA1-AB5E-DCFEF04AF245}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3032125" y="412750"/>
+              <a:ext cx="4152900" cy="1254125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="16355C"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Ndv</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t> (</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>i ==&gt; (n/v)_i):</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>  T</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>he ratio obtained by dividing the engine speed n by the vehicle speed v for each gear i, for i to ng max , </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSup>
+                    <m:sSupPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="es-ES" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="bg1"/>
+                          </a:solidFill>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSupPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="es-ES" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="bg1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑚𝑖𝑛</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sup>
+                      <m:r>
+                        <a:rPr lang="es-ES" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="bg1"/>
+                          </a:solidFill>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>−1</m:t>
+                      </m:r>
+                    </m:sup>
+                  </m:sSup>
+                  <m:r>
+                    <a:rPr lang="es-ES" sz="1200" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>/(</m:t>
+                  </m:r>
+                  <m:f>
+                    <m:fPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="es-ES" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="bg1"/>
+                          </a:solidFill>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:fPr>
+                    <m:num>
+                      <m:r>
+                        <a:rPr lang="es-ES" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="bg1"/>
+                          </a:solidFill>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑘𝑚</m:t>
+                      </m:r>
+                    </m:num>
+                    <m:den>
+                      <m:r>
+                        <a:rPr lang="es-ES" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="bg1"/>
+                          </a:solidFill>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>h</m:t>
+                      </m:r>
+                    </m:den>
+                  </m:f>
+                  <m:r>
+                    <a:rPr lang="es-ES" sz="1200" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>)</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>. </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="es-ES_tradnl" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="bg1"/>
+                          </a:solidFill>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:d>
+                        <m:dPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="es-ES_tradnl" sz="1100" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="bg1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:dPr>
+                        <m:e>
+                          <m:f>
+                            <m:fPr>
+                              <m:ctrlPr>
+                                <a:rPr lang="es-ES_tradnl" sz="1100" b="0" i="1">
+                                  <a:solidFill>
+                                    <a:schemeClr val="bg1"/>
+                                  </a:solidFill>
+                                  <a:effectLst/>
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  <a:ea typeface="+mn-ea"/>
+                                  <a:cs typeface="+mn-cs"/>
+                                </a:rPr>
+                              </m:ctrlPr>
+                            </m:fPr>
+                            <m:num>
+                              <m:r>
+                                <a:rPr lang="es-ES" sz="1100" b="0" i="1">
+                                  <a:solidFill>
+                                    <a:schemeClr val="bg1"/>
+                                  </a:solidFill>
+                                  <a:effectLst/>
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  <a:ea typeface="+mn-ea"/>
+                                  <a:cs typeface="+mn-cs"/>
+                                </a:rPr>
+                                <m:t>𝑛</m:t>
+                              </m:r>
+                            </m:num>
+                            <m:den>
+                              <m:r>
+                                <a:rPr lang="es-ES" sz="1100" b="0" i="1">
+                                  <a:solidFill>
+                                    <a:schemeClr val="bg1"/>
+                                  </a:solidFill>
+                                  <a:effectLst/>
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  <a:ea typeface="+mn-ea"/>
+                                  <a:cs typeface="+mn-cs"/>
+                                </a:rPr>
+                                <m:t>𝑣</m:t>
+                              </m:r>
+                            </m:den>
+                          </m:f>
+                        </m:e>
+                      </m:d>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="es-ES" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="bg1"/>
+                          </a:solidFill>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑖</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t> shall be calculated using the equations in paragraph 8. of Sub-Annex 7; [Ref: Paragraph 2, point e of Sub-Annex 2]</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="CuadroTexto 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BB209E8-E9D6-4FA1-AB5E-DCFEF04AF245}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3032125" y="412750"/>
+              <a:ext cx="4152900" cy="1254125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="16355C"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Ndv</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t> (</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>i ==&gt; (n/v)_i):</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>  T</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>he ratio obtained by dividing the engine speed n by the vehicle speed v for each gear i, for i to ng max , </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑚𝑖𝑛</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>〗^(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−1)/(𝑘𝑚/ℎ)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>. </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑛</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES_tradnl" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>

</xml_diff>

<commit_message>
update(demos): New format for the input files.
</commit_message>
<xml_diff>
--- a/gearshift/demos/gs_input_demo_empty.xlsx
+++ b/gearshift/demos/gs_input_demo_empty.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\European Comision\WLTP\gearshift_calculation_tool\gearshift\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FE6E65-CA44-438E-880F-596B37793F17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E318F730-F2A4-46C8-8C29-DEF143B85600}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5C24A396-E983-DB47-8B10-835CCBF80F80}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <definedName name="case" localSheetId="1">case!$A$1:$V$3</definedName>
     <definedName name="engine" localSheetId="3">engine!$A$1:$D$5097</definedName>
     <definedName name="gearbox" localSheetId="4">gearbox_ratios!$A$1:$C$652</definedName>
-    <definedName name="vehicle" localSheetId="2">vehicle!$A$1:$J$118</definedName>
+    <definedName name="vehicle" localSheetId="2">vehicle!$A$1:$I$118</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -492,9 +492,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -630,32 +637,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
@@ -669,15 +678,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -685,48 +694,56 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{44E1B410-3729-2B4E-8A43-D351FD98412A}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{7174B9F6-3876-4674-A2BC-A9F367224990}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{9EF088D8-80F1-4ED1-82D9-5D9B5F9E7184}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1755,15 +1772,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>177801</xdr:rowOff>
+      <xdr:rowOff>187326</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:colOff>34925</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1778,7 +1795,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7324725" y="377826"/>
+          <a:off x="7334250" y="387351"/>
           <a:ext cx="6731000" cy="6394450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4732,601 +4749,601 @@
     </row>
     <row r="15" spans="1:15" s="17" customFormat="1"/>
     <row r="16" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
     </row>
     <row r="18" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
     </row>
     <row r="19" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
     </row>
     <row r="20" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
     </row>
     <row r="21" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
     </row>
     <row r="22" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
     </row>
     <row r="23" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
     </row>
     <row r="24" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
     </row>
     <row r="25" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
     </row>
     <row r="26" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
     </row>
     <row r="27" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
     </row>
     <row r="28" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
     </row>
     <row r="29" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="25"/>
     </row>
     <row r="30" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="25"/>
     </row>
     <row r="31" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="25"/>
     </row>
     <row r="32" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
     </row>
     <row r="33" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="25"/>
     </row>
     <row r="34" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
     </row>
     <row r="35" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="23"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
     </row>
     <row r="36" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
     </row>
     <row r="37" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A37" s="23"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="23"/>
-      <c r="N37" s="23"/>
-      <c r="O37" s="23"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="25"/>
+      <c r="O37" s="25"/>
     </row>
     <row r="38" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A38" s="23"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="23"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="25"/>
+      <c r="N38" s="25"/>
+      <c r="O38" s="25"/>
     </row>
     <row r="39" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="23"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="23"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
     </row>
     <row r="40" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="23"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="23"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="23"/>
-      <c r="M40" s="23"/>
-      <c r="N40" s="23"/>
-      <c r="O40" s="23"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
     </row>
     <row r="41" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A41" s="23"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="23"/>
-      <c r="N41" s="23"/>
-      <c r="O41" s="23"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+      <c r="O41" s="25"/>
     </row>
     <row r="42" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25"/>
     </row>
     <row r="43" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="23"/>
-      <c r="N43" s="23"/>
-      <c r="O43" s="23"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25"/>
+      <c r="O43" s="25"/>
     </row>
     <row r="44" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="25"/>
+      <c r="O44" s="25"/>
     </row>
     <row r="45" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="23"/>
-      <c r="N45" s="23"/>
-      <c r="O45" s="23"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25"/>
+      <c r="L45" s="25"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="25"/>
+      <c r="O45" s="25"/>
     </row>
     <row r="46" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="23"/>
-      <c r="M46" s="23"/>
-      <c r="N46" s="23"/>
-      <c r="O46" s="23"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="25"/>
+      <c r="L46" s="25"/>
+      <c r="M46" s="25"/>
+      <c r="N46" s="25"/>
+      <c r="O46" s="25"/>
     </row>
     <row r="47" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A47" s="23"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="23"/>
-      <c r="L47" s="23"/>
-      <c r="M47" s="23"/>
-      <c r="N47" s="23"/>
-      <c r="O47" s="23"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="25"/>
+      <c r="J47" s="25"/>
+      <c r="K47" s="25"/>
+      <c r="L47" s="25"/>
+      <c r="M47" s="25"/>
+      <c r="N47" s="25"/>
+      <c r="O47" s="25"/>
     </row>
     <row r="48" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="23"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="23"/>
-      <c r="L48" s="23"/>
-      <c r="M48" s="23"/>
-      <c r="N48" s="23"/>
-      <c r="O48" s="23"/>
+      <c r="A48" s="25"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="25"/>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25"/>
+      <c r="M48" s="25"/>
+      <c r="N48" s="25"/>
+      <c r="O48" s="25"/>
     </row>
     <row r="49" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A49" s="23"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="23"/>
-      <c r="M49" s="23"/>
-      <c r="N49" s="23"/>
-      <c r="O49" s="23"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="25"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="25"/>
+      <c r="M49" s="25"/>
+      <c r="N49" s="25"/>
+      <c r="O49" s="25"/>
     </row>
     <row r="50" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A50" s="23"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="23"/>
-      <c r="L50" s="23"/>
-      <c r="M50" s="23"/>
-      <c r="N50" s="23"/>
-      <c r="O50" s="23"/>
+      <c r="A50" s="25"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
+      <c r="K50" s="25"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="25"/>
+      <c r="N50" s="25"/>
+      <c r="O50" s="25"/>
     </row>
     <row r="51" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
       <c r="A51" s="19"/>
@@ -5476,10 +5493,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -5640,9 +5657,17 @@
         <v>46</v>
       </c>
     </row>
+    <row r="3" spans="1:22">
+      <c r="E3" s="23"/>
+    </row>
   </sheetData>
-  <sheetProtection sheet="1" scenarios="1" insertRows="0"/>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <sheetProtection insertRows="0" deleteRows="0"/>
+  <phoneticPr fontId="11" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3 E4:E2780" xr:uid="{98515D48-B5A1-4177-98DC-437651B329F0}">
+      <formula1>"class 1,class 2,class 3a,class 3b"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -5657,19 +5682,19 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J3" sqref="A3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="8" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.625" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="11" style="9"/>
   </cols>
   <sheetData>
@@ -5687,22 +5712,22 @@
         <v>22</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -5719,29 +5744,29 @@
         <v>29</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8">
-      <c r="H37" s="13"/>
+    </row>
+    <row r="37" spans="7:7">
+      <c r="G37" s="13"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" scenarios="1" insertRows="0"/>
+  <sheetProtection sheet="1" scenarios="1" insertRows="0" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -5753,10 +5778,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -5796,9 +5821,233 @@
         <v>42</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+    </row>
   </sheetData>
-  <sheetProtection sheet="1" scenarios="1"/>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <sheetProtection sheet="1" scenarios="1" deleteRows="0"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5812,7 +6061,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -5846,7 +6095,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" scenarios="1"/>
+  <sheetProtection sheet="1" scenarios="1" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update(demo files): Update excel demo files with the new logo.
</commit_message>
<xml_diff>
--- a/gearshift/demos/gs_input_demo_empty.xlsx
+++ b/gearshift/demos/gs_input_demo_empty.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\European Comision\WLTP\gearshift_calculation_tool\gearshift\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E318F730-F2A4-46C8-8C29-DEF143B85600}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D43BAA-B429-4EFB-B591-A9F8DBCD434E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5C24A396-E983-DB47-8B10-835CCBF80F80}"/>
   </bookViews>
   <sheets>
-    <sheet name="About" sheetId="10" r:id="rId1"/>
+    <sheet name="About" sheetId="13" r:id="rId1"/>
     <sheet name="case" sheetId="1" r:id="rId2"/>
     <sheet name="vehicle" sheetId="2" r:id="rId3"/>
     <sheet name="engine" sheetId="12" r:id="rId4"/>
@@ -492,9 +492,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -637,34 +644,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
@@ -678,15 +682,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -694,55 +698,60 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="4" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{44E1B410-3729-2B4E-8A43-D351FD98412A}"/>
     <cellStyle name="Normal 2 2" xfId="2" xr:uid="{7174B9F6-3876-4674-A2BC-A9F367224990}"/>
+    <cellStyle name="Normal 2 2 2" xfId="4" xr:uid="{34571906-AAFD-4161-9569-B806114C1230}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{9EF088D8-80F1-4ED1-82D9-5D9B5F9E7184}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -765,25 +774,83 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>6804</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>6804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>90714</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectángulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1A4372A-4076-4DFD-9853-4BE17387C892}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6804" y="6804"/>
+          <a:ext cx="10423071" cy="2850696"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>632732</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142883</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7772400" cy="736332"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagen 5">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFCC2C72-54C0-A04E-A64C-4CF9B752058C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46718819-7DED-44E5-9FEB-AA9CE6A80F3D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -792,7 +859,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -805,8 +872,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="10477500" cy="2757714"/>
+          <a:off x="1328057" y="1095383"/>
+          <a:ext cx="7772400" cy="736332"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -814,7 +881,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4495,986 +4562,986 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3C2E93-7C6E-7147-8A63-5B38643369BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD104AF8-09F5-4F9B-A77D-E558BCD3734F}">
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:O50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="15" width="9.125" style="17" customWidth="1"/>
-    <col min="16" max="16" width="9.125" style="16" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.125" style="16" hidden="1"/>
+    <col min="1" max="15" width="9.125" style="18" customWidth="1"/>
+    <col min="16" max="16" width="9.125" style="17" hidden="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.125" style="17" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-    </row>
-    <row r="15" spans="1:15" s="17" customFormat="1"/>
-    <row r="16" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="24" t="s">
+    <row r="1" spans="1:15" ht="15">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" ht="15">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+    </row>
+    <row r="3" spans="1:15" ht="15">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+    </row>
+    <row r="4" spans="1:15" ht="15">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+    </row>
+    <row r="5" spans="1:15" ht="15">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+    </row>
+    <row r="6" spans="1:15" ht="15">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+    </row>
+    <row r="7" spans="1:15" ht="15">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+    </row>
+    <row r="8" spans="1:15" ht="15">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+    </row>
+    <row r="9" spans="1:15" ht="15">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+    </row>
+    <row r="10" spans="1:15" ht="15">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+    </row>
+    <row r="11" spans="1:15" ht="15">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+    </row>
+    <row r="12" spans="1:15" ht="15">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+    </row>
+    <row r="13" spans="1:15" ht="15">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+    </row>
+    <row r="14" spans="1:15" ht="15">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+    </row>
+    <row r="15" spans="1:15" s="18" customFormat="1" ht="15"/>
+    <row r="16" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A16" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-    </row>
-    <row r="17" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-    </row>
-    <row r="18" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-    </row>
-    <row r="19" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="25"/>
-    </row>
-    <row r="20" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-    </row>
-    <row r="21" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-    </row>
-    <row r="22" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-    </row>
-    <row r="23" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-    </row>
-    <row r="24" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-    </row>
-    <row r="25" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-    </row>
-    <row r="26" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-    </row>
-    <row r="27" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-    </row>
-    <row r="28" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-    </row>
-    <row r="29" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-    </row>
-    <row r="30" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-    </row>
-    <row r="31" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-    </row>
-    <row r="32" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="25"/>
-    </row>
-    <row r="33" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="25"/>
-    </row>
-    <row r="34" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25"/>
-    </row>
-    <row r="35" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-    </row>
-    <row r="36" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-    </row>
-    <row r="37" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="25"/>
-    </row>
-    <row r="38" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="25"/>
-    </row>
-    <row r="39" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="25"/>
-      <c r="O39" s="25"/>
-    </row>
-    <row r="40" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="25"/>
-    </row>
-    <row r="41" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A41" s="25"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="25"/>
-    </row>
-    <row r="42" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="25"/>
-      <c r="N42" s="25"/>
-      <c r="O42" s="25"/>
-    </row>
-    <row r="43" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="25"/>
-      <c r="O43" s="25"/>
-    </row>
-    <row r="44" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
-      <c r="L44" s="25"/>
-      <c r="M44" s="25"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="25"/>
-    </row>
-    <row r="45" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="25"/>
-      <c r="O45" s="25"/>
-    </row>
-    <row r="46" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="25"/>
-      <c r="N46" s="25"/>
-      <c r="O46" s="25"/>
-    </row>
-    <row r="47" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="25"/>
-      <c r="N47" s="25"/>
-      <c r="O47" s="25"/>
-    </row>
-    <row r="48" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="25"/>
-      <c r="N48" s="25"/>
-      <c r="O48" s="25"/>
-    </row>
-    <row r="49" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
-      <c r="N49" s="25"/>
-      <c r="O49" s="25"/>
-    </row>
-    <row r="50" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="25"/>
-      <c r="J50" s="25"/>
-      <c r="K50" s="25"/>
-      <c r="L50" s="25"/>
-      <c r="M50" s="25"/>
-      <c r="N50" s="25"/>
-      <c r="O50" s="25"/>
-    </row>
-    <row r="51" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A51" s="19"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="19"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="19"/>
-      <c r="N51" s="19"/>
-      <c r="O51" s="19"/>
-    </row>
-    <row r="52" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A52" s="19"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="19"/>
-      <c r="L52" s="19"/>
-      <c r="M52" s="19"/>
-      <c r="N52" s="19"/>
-      <c r="O52" s="19"/>
-    </row>
-    <row r="53" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A53" s="19"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19"/>
-      <c r="L53" s="19"/>
-      <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
-      <c r="O53" s="19"/>
-    </row>
-    <row r="54" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A54" s="19"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
-      <c r="J54" s="19"/>
-      <c r="K54" s="19"/>
-      <c r="L54" s="19"/>
-      <c r="M54" s="19"/>
-      <c r="N54" s="19"/>
-      <c r="O54" s="19"/>
-    </row>
-    <row r="55" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A55" s="19"/>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19"/>
-      <c r="L55" s="19"/>
-      <c r="M55" s="19"/>
-      <c r="N55" s="19"/>
-      <c r="O55" s="19"/>
-    </row>
-    <row r="56" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1">
-      <c r="A56" s="19"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="19"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="19"/>
-      <c r="M56" s="19"/>
-      <c r="N56" s="19"/>
-      <c r="O56" s="19"/>
-    </row>
-    <row r="57" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
-      <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="20"/>
-      <c r="J57" s="20"/>
-      <c r="K57" s="20"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="20"/>
-      <c r="N57" s="20"/>
-      <c r="O57" s="20"/>
-    </row>
-    <row r="61" spans="1:15" hidden="1">
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="1:15" hidden="1">
-      <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="1:15" hidden="1">
-      <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="1:15" hidden="1">
-      <c r="B64" s="1"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+    </row>
+    <row r="17" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+    </row>
+    <row r="18" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+    </row>
+    <row r="19" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+    </row>
+    <row r="20" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+    </row>
+    <row r="21" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+    </row>
+    <row r="22" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+    </row>
+    <row r="23" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+    </row>
+    <row r="24" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+    </row>
+    <row r="25" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+    </row>
+    <row r="26" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+    </row>
+    <row r="27" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+    </row>
+    <row r="28" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+    </row>
+    <row r="29" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+    </row>
+    <row r="30" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+    </row>
+    <row r="31" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+    </row>
+    <row r="32" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+    </row>
+    <row r="33" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+    </row>
+    <row r="34" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+    </row>
+    <row r="35" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+    </row>
+    <row r="36" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+    </row>
+    <row r="37" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+    </row>
+    <row r="38" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A38" s="20"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+    </row>
+    <row r="39" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+    </row>
+    <row r="40" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A40" s="20"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+    </row>
+    <row r="41" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+    </row>
+    <row r="42" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A42" s="20"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+    </row>
+    <row r="43" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="20"/>
+      <c r="O43" s="20"/>
+    </row>
+    <row r="44" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+    </row>
+    <row r="45" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="20"/>
+      <c r="O45" s="20"/>
+    </row>
+    <row r="46" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A46" s="20"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+      <c r="N46" s="20"/>
+      <c r="O46" s="20"/>
+    </row>
+    <row r="47" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="20"/>
+    </row>
+    <row r="48" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A48" s="20"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="20"/>
+      <c r="O48" s="20"/>
+    </row>
+    <row r="49" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="20"/>
+      <c r="O49" s="20"/>
+    </row>
+    <row r="50" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="20"/>
+      <c r="O50" s="20"/>
+    </row>
+    <row r="51" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A51" s="22"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
+    </row>
+    <row r="52" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A52" s="22"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="22"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="22"/>
+    </row>
+    <row r="53" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A53" s="22"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="22"/>
+      <c r="L53" s="22"/>
+      <c r="M53" s="22"/>
+      <c r="N53" s="22"/>
+      <c r="O53" s="22"/>
+    </row>
+    <row r="54" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="22"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="22"/>
+      <c r="N54" s="22"/>
+      <c r="O54" s="22"/>
+    </row>
+    <row r="55" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A55" s="22"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
+      <c r="K55" s="22"/>
+      <c r="L55" s="22"/>
+      <c r="M55" s="22"/>
+      <c r="N55" s="22"/>
+      <c r="O55" s="22"/>
+    </row>
+    <row r="56" spans="1:15" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A56" s="22"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="22"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="22"/>
+      <c r="K56" s="22"/>
+      <c r="L56" s="22"/>
+      <c r="M56" s="22"/>
+      <c r="N56" s="22"/>
+      <c r="O56" s="22"/>
+    </row>
+    <row r="57" spans="1:15" s="24" customFormat="1" ht="15" customHeight="1">
+      <c r="A57" s="23"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="23"/>
+      <c r="L57" s="23"/>
+      <c r="M57" s="23"/>
+      <c r="N57" s="23"/>
+      <c r="O57" s="23"/>
+    </row>
+    <row r="61" spans="1:15" ht="15" hidden="1">
+      <c r="B61" s="25"/>
+    </row>
+    <row r="62" spans="1:15" ht="15" hidden="1">
+      <c r="B62" s="25"/>
+    </row>
+    <row r="63" spans="1:15" ht="15" hidden="1">
+      <c r="B63" s="25"/>
+    </row>
+    <row r="64" spans="1:15" ht="15" hidden="1">
+      <c r="B64" s="25"/>
     </row>
     <row r="65" ht="15" customHeight="1"/>
   </sheetData>
@@ -5501,168 +5568,168 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="7" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="6.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11" style="9"/>
+    <col min="1" max="1" width="7" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="6.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:22" s="3" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="6" customFormat="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:22" s="5" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:22">
-      <c r="E3" s="23"/>
+      <c r="E3" s="16"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" deleteRows="0"/>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3 E4:E2780" xr:uid="{98515D48-B5A1-4177-98DC-437651B329F0}">
       <formula1>"class 1,class 2,class 3a,class 3b"</formula1>
@@ -5687,83 +5754,83 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="8" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11" style="9"/>
+    <col min="1" max="2" width="8" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:10" s="7" customFormat="1">
+      <c r="A1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="13"/>
+      <c r="G37" s="12"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" scenarios="1" insertRows="0" deleteRows="0"/>
@@ -5786,268 +5853,268 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="7" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11" style="9"/>
+    <col min="1" max="1" width="7" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
     </row>
     <row r="18" spans="2:3">
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
     </row>
     <row r="20" spans="2:3">
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
     </row>
     <row r="21" spans="2:3">
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
     </row>
     <row r="22" spans="2:3">
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
     </row>
     <row r="23" spans="2:3">
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
     </row>
     <row r="24" spans="2:3">
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="2:3">
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
     </row>
     <row r="26" spans="2:3">
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
     </row>
     <row r="28" spans="2:3">
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" spans="2:3">
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
     </row>
     <row r="30" spans="2:3">
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" spans="2:3">
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
     </row>
     <row r="32" spans="2:3">
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
     </row>
     <row r="33" spans="2:3">
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
     </row>
     <row r="34" spans="2:3">
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
     </row>
     <row r="35" spans="2:3">
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" spans="2:3">
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
     </row>
     <row r="37" spans="2:3">
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
     </row>
     <row r="38" spans="2:3">
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
     </row>
     <row r="39" spans="2:3">
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
     </row>
     <row r="40" spans="2:3">
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
     </row>
     <row r="41" spans="2:3">
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
     </row>
     <row r="42" spans="2:3">
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
     </row>
     <row r="43" spans="2:3">
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
     </row>
     <row r="44" spans="2:3">
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
     </row>
     <row r="45" spans="2:3">
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
     </row>
     <row r="46" spans="2:3">
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
     </row>
     <row r="47" spans="2:3">
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
     </row>
     <row r="48" spans="2:3">
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
     </row>
     <row r="49" spans="2:3">
-      <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
     </row>
     <row r="50" spans="2:3">
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
     </row>
     <row r="51" spans="2:3">
-      <c r="B51" s="22"/>
-      <c r="C51" s="22"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
     </row>
     <row r="52" spans="2:3">
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
     </row>
     <row r="53" spans="2:3">
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
     </row>
     <row r="54" spans="2:3">
-      <c r="B54" s="22"/>
-      <c r="C54" s="22"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
     </row>
     <row r="55" spans="2:3">
-      <c r="B55" s="22"/>
-      <c r="C55" s="22"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
     </row>
     <row r="56" spans="2:3">
-      <c r="B56" s="22"/>
-      <c r="C56" s="22"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
     </row>
     <row r="57" spans="2:3">
-      <c r="B57" s="22"/>
-      <c r="C57" s="22"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
     </row>
     <row r="58" spans="2:3">
-      <c r="B58" s="22"/>
-      <c r="C58" s="22"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" scenarios="1" deleteRows="0"/>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6066,31 +6133,31 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11" style="9"/>
+    <col min="1" max="1" width="7.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>